<commit_message>
[Doc] Update Entwurf, Pflichtenheft
</commit_message>
<xml_diff>
--- a/Dokumentation/Projektkalender.xlsx
+++ b/Dokumentation/Projektkalender.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicole\Documents\GitHub\TeeShop_soft\Dokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BD44202-1EEA-4A35-A6AA-7D7AAD8BB4C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6FFFC72-A130-4929-B583-B955E428BA17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16330" yWindow="5010" windowWidth="28800" windowHeight="15420" xr2:uid="{703252D3-C12B-466E-8ACC-15D787E6709C}"/>
+    <workbookView xWindow="12640" yWindow="3510" windowWidth="28800" windowHeight="15420" xr2:uid="{703252D3-C12B-466E-8ACC-15D787E6709C}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="68">
   <si>
     <t>PROJEKTTITEL:</t>
   </si>
@@ -91,52 +91,21 @@
     <t>1.3</t>
   </si>
   <si>
-    <t>Ideensammlung 
-(Entwurf, Funktion)</t>
-  </si>
-  <si>
     <t>1.4</t>
   </si>
   <si>
     <t>Projektbearbeitung</t>
   </si>
   <si>
-    <t>2.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Website-Layout </t>
-  </si>
-  <si>
     <t>Anna Bacinscaia</t>
   </si>
   <si>
-    <t>2.2</t>
-  </si>
-  <si>
     <t>Datenbank anlegen</t>
   </si>
   <si>
     <t>Erik Grüneberger, Paul Leon Weber</t>
   </si>
   <si>
-    <t>2.11</t>
-  </si>
-  <si>
-    <t>2.12</t>
-  </si>
-  <si>
-    <t>2.13</t>
-  </si>
-  <si>
-    <t>2.14</t>
-  </si>
-  <si>
-    <t>2.15</t>
-  </si>
-  <si>
-    <t>2.16</t>
-  </si>
-  <si>
     <t>Projektdokumentation</t>
   </si>
   <si>
@@ -179,9 +148,6 @@
     <t>UML-Diagramme</t>
   </si>
   <si>
-    <t>2.17</t>
-  </si>
-  <si>
     <t>Layout Startseite</t>
   </si>
   <si>
@@ -210,6 +176,72 @@
   </si>
   <si>
     <t>Fehlerbehebung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ideensammlung </t>
+  </si>
+  <si>
+    <t>Layout "Produkt anlegen"</t>
+  </si>
+  <si>
+    <t>Layout "Kategorie anlegen"</t>
+  </si>
+  <si>
+    <t>Layout "Produkt bearbeiten"</t>
+  </si>
+  <si>
+    <t>Layout "Kategorie bearbeiten"</t>
+  </si>
+  <si>
+    <t>2.1.1</t>
+  </si>
+  <si>
+    <t>2.1.2</t>
+  </si>
+  <si>
+    <t>2.1.3</t>
+  </si>
+  <si>
+    <t>2.1.4</t>
+  </si>
+  <si>
+    <t>2.1.5</t>
+  </si>
+  <si>
+    <t>2.1.6</t>
+  </si>
+  <si>
+    <t>2.1.7</t>
+  </si>
+  <si>
+    <t>2.1.8</t>
+  </si>
+  <si>
+    <t>2.1.9</t>
+  </si>
+  <si>
+    <t>2.1.10</t>
+  </si>
+  <si>
+    <t>2.1.11</t>
+  </si>
+  <si>
+    <t>2.2.1</t>
+  </si>
+  <si>
+    <t>Datenbankstruktur erstellen</t>
+  </si>
+  <si>
+    <t>Website-Entwurf</t>
+  </si>
+  <si>
+    <t>2.2.2</t>
+  </si>
+  <si>
+    <t>2.3</t>
+  </si>
+  <si>
+    <t>2.4</t>
   </si>
 </sst>
 </file>
@@ -383,6 +415,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -391,7 +424,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -709,22 +741,22 @@
   <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="32.6328125" customWidth="1"/>
+    <col min="2" max="2" width="34.54296875" customWidth="1"/>
     <col min="3" max="3" width="41.36328125" customWidth="1"/>
     <col min="4" max="4" width="33.36328125" customWidth="1"/>
     <col min="5" max="5" width="24.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
+      <c r="B1" s="14"/>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
@@ -732,10 +764,10 @@
       <c r="E1" s="2"/>
     </row>
     <row r="2" spans="1:5" ht="27.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="15"/>
+      <c r="B2" s="16"/>
       <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
@@ -793,7 +825,7 @@
         <v>44638</v>
       </c>
       <c r="E6" s="9">
-        <v>44638</v>
+        <v>44657</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.35">
@@ -809,14 +841,16 @@
       <c r="D7" s="9">
         <v>44649</v>
       </c>
-      <c r="E7" s="9"/>
+      <c r="E7" s="9">
+        <v>44665</v>
+      </c>
     </row>
     <row r="8" spans="1:5" ht="39" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="9" t="s">
         <v>16</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>13</v>
@@ -824,23 +858,33 @@
       <c r="D8" s="9">
         <v>44650</v>
       </c>
-      <c r="E8" s="9"/>
+      <c r="E8" s="9">
+        <v>44658</v>
+      </c>
     </row>
     <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.35">
       <c r="A9" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
+        <v>17</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="9">
+        <v>44641</v>
+      </c>
+      <c r="E9" s="9">
+        <v>44658</v>
+      </c>
     </row>
     <row r="10" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="6">
         <v>2</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
@@ -848,173 +892,202 @@
     </row>
     <row r="11" spans="1:5" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="10" t="s">
-        <v>20</v>
+        <v>51</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D11" s="9">
-        <v>44650</v>
-      </c>
-      <c r="E11" s="9"/>
+        <v>44651</v>
+      </c>
+      <c r="E11" s="9">
+        <v>44655</v>
+      </c>
     </row>
     <row r="12" spans="1:5" ht="24.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="10" t="s">
-        <v>26</v>
+        <v>52</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D12" s="9">
-        <v>44651</v>
+        <v>44662</v>
       </c>
       <c r="E12" s="9"/>
     </row>
     <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.35">
       <c r="A13" s="10" t="s">
-        <v>27</v>
+        <v>53</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" s="9">
-        <v>44655</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="D13" s="9"/>
       <c r="E13" s="9"/>
     </row>
     <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.35">
       <c r="A14" s="10" t="s">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D14" s="9"/>
       <c r="E14" s="9"/>
     </row>
     <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.35">
       <c r="A15" s="10" t="s">
-        <v>29</v>
+        <v>55</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D15" s="9"/>
       <c r="E15" s="9"/>
     </row>
     <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.35">
       <c r="A16" s="10" t="s">
-        <v>30</v>
+        <v>56</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D16" s="9"/>
       <c r="E16" s="9"/>
     </row>
     <row r="17" spans="1:5" ht="15" x14ac:dyDescent="0.35">
       <c r="A17" s="10" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D17" s="9"/>
+        <v>19</v>
+      </c>
+      <c r="D17" s="12"/>
       <c r="E17" s="9"/>
     </row>
     <row r="18" spans="1:5" ht="15" x14ac:dyDescent="0.35">
       <c r="A18" s="10" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D18" s="16"/>
+        <v>19</v>
+      </c>
+      <c r="D18" s="12"/>
       <c r="E18" s="9"/>
     </row>
     <row r="19" spans="1:5" ht="15" x14ac:dyDescent="0.35">
       <c r="A19" s="10" t="s">
-        <v>23</v>
+        <v>59</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="D19" s="9">
+        <v>19</v>
+      </c>
+      <c r="D19" s="12"/>
+      <c r="E19" s="9"/>
+    </row>
+    <row r="20" spans="1:5" ht="15" x14ac:dyDescent="0.35">
+      <c r="A20" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20" s="12"/>
+      <c r="E20" s="9"/>
+    </row>
+    <row r="21" spans="1:5" ht="15" x14ac:dyDescent="0.35">
+      <c r="A21" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+    </row>
+    <row r="22" spans="1:5" ht="15" x14ac:dyDescent="0.35">
+      <c r="A22" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D22" s="9">
         <v>44650</v>
       </c>
-      <c r="E19" s="9"/>
-    </row>
-    <row r="20" spans="1:5" ht="15" x14ac:dyDescent="0.35">
-      <c r="A20" s="10"/>
-      <c r="B20" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="C20" s="11"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-    </row>
-    <row r="21" spans="1:5" ht="15" x14ac:dyDescent="0.35">
-      <c r="A21" s="10"/>
-      <c r="B21" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="C21" s="11"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="9"/>
-    </row>
-    <row r="22" spans="1:5" ht="15" x14ac:dyDescent="0.35">
-      <c r="A22" s="10"/>
-      <c r="B22" s="11"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
+      <c r="E22" s="9">
+        <v>44658</v>
+      </c>
     </row>
     <row r="23" spans="1:5" ht="15" x14ac:dyDescent="0.35">
-      <c r="A23" s="10"/>
-      <c r="B23" s="16"/>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16"/>
+      <c r="A23" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>21</v>
+      </c>
       <c r="E23" s="9"/>
     </row>
     <row r="24" spans="1:5" ht="15" x14ac:dyDescent="0.35">
-      <c r="A24" s="10"/>
-      <c r="B24" s="11"/>
+      <c r="A24" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>44</v>
+      </c>
       <c r="C24" s="11"/>
       <c r="D24" s="9"/>
       <c r="E24" s="9"/>
     </row>
     <row r="25" spans="1:5" ht="15" x14ac:dyDescent="0.35">
-      <c r="A25" s="10"/>
-      <c r="B25" s="11"/>
+      <c r="A25" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>45</v>
+      </c>
       <c r="C25" s="11"/>
-      <c r="D25" s="9"/>
+      <c r="D25" s="12"/>
       <c r="E25" s="9"/>
     </row>
     <row r="26" spans="1:5" ht="15" x14ac:dyDescent="0.35">
@@ -1029,7 +1102,7 @@
         <v>3</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="C27" s="6"/>
       <c r="D27" s="7"/>
@@ -1037,13 +1110,13 @@
     </row>
     <row r="28" spans="1:5" ht="40" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="10" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="D28" s="9">
         <v>44650</v>
@@ -1052,13 +1125,13 @@
     </row>
     <row r="29" spans="1:5" ht="41.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="10" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="D29" s="9">
         <v>44651</v>
@@ -1067,10 +1140,10 @@
     </row>
     <row r="30" spans="1:5" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="10" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="C30" s="9"/>
       <c r="D30" s="9"/>
@@ -1078,13 +1151,13 @@
     </row>
     <row r="31" spans="1:5" ht="15" x14ac:dyDescent="0.35">
       <c r="A31" s="10" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="D31" s="9">
         <v>44656</v>
@@ -1093,10 +1166,10 @@
     </row>
     <row r="32" spans="1:5" ht="15" x14ac:dyDescent="0.35">
       <c r="A32" s="10" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="C32" s="9"/>
       <c r="D32" s="9"/>
@@ -1104,7 +1177,7 @@
     </row>
     <row r="33" spans="1:5" ht="15" x14ac:dyDescent="0.35">
       <c r="A33" s="10" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="B33" s="9"/>
       <c r="C33" s="9"/>
@@ -1113,7 +1186,7 @@
     </row>
     <row r="34" spans="1:5" ht="15" x14ac:dyDescent="0.35">
       <c r="A34" s="10" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B34" s="9"/>
       <c r="C34" s="9"/>
@@ -1122,7 +1195,7 @@
     </row>
     <row r="35" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="10" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="B35" s="9"/>
       <c r="C35" s="9"/>

</xml_diff>